<commit_message>
Update steps using unordered lists
</commit_message>
<xml_diff>
--- a/testit.xlsx
+++ b/testit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519F3E95-7A9A-4025-95D2-01965E5802A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB840E2-3E3E-4871-987D-FEA46C090126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24525" yWindow="5985" windowWidth="21600" windowHeight="11385" tabRatio="618" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="28">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -82,11 +82,6 @@
   </si>
   <si>
     <t>t1</t>
-  </si>
-  <si>
-    <t>do this
-do that
-and this and that</t>
   </si>
   <si>
     <t>P</t>
@@ -487,7 +482,7 @@
   <dimension ref="B3:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +499,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>2</v>
@@ -513,7 +508,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>4</v>
@@ -542,13 +537,13 @@
         <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
@@ -564,10 +559,10 @@
         <v>12</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="1"/>
     </row>
@@ -584,7 +579,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>0</v>
@@ -593,7 +588,7 @@
     </row>
     <row r="7" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
@@ -608,13 +603,13 @@
         <v>12</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.25">
@@ -640,17 +635,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A37B09-C095-48EF-9951-3AAF0C506CDF}">
-  <dimension ref="B3:I7"/>
+  <dimension ref="B3:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="24.42578125" customWidth="1"/>
   </cols>
@@ -660,7 +655,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>2</v>
@@ -669,7 +664,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>4</v>
@@ -683,7 +678,7 @@
     </row>
     <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -698,18 +693,18 @@
         <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -720,16 +715,16 @@
         <v>12</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -740,7 +735,7 @@
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>0</v>
@@ -749,7 +744,7 @@
     </row>
     <row r="7" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
@@ -764,13 +759,28 @@
         <v>12</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>17</v>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -780,17 +790,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C33F8E10-6F2B-46E4-B593-C41A35710CA3}">
-  <dimension ref="B3:I7"/>
+  <dimension ref="B3:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16.42578125" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="24.42578125" customWidth="1"/>
   </cols>
@@ -800,7 +810,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>2</v>
@@ -809,7 +819,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>4</v>
@@ -823,7 +833,7 @@
     </row>
     <row r="4" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -838,18 +848,18 @@
         <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -860,16 +870,16 @@
         <v>12</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -880,16 +890,16 @@
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="2:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>8</v>
@@ -904,13 +914,28 @@
         <v>12</v>
       </c>
       <c r="G7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>17</v>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>